<commit_message>
Lavet funktionsliste, opdateret ordre med ekstra bemærkning
</commit_message>
<xml_diff>
--- a/System udvikling/Funktionsliste.xlsx
+++ b/System udvikling/Funktionsliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Funktionsliste</t>
   </si>
@@ -48,15 +48,6 @@
     <t>Opret provisionssedler og kontoudtog</t>
   </si>
   <si>
-    <t>Print faktura/ordre</t>
-  </si>
-  <si>
-    <t>Email faktura/ordre</t>
-  </si>
-  <si>
-    <t>Eksporter/Importer kommaseparerede filer</t>
-  </si>
-  <si>
     <t>Simpel</t>
   </si>
   <si>
@@ -66,9 +57,6 @@
     <t>Kompleks</t>
   </si>
   <si>
-    <t>Ændr konstant</t>
-  </si>
-  <si>
     <t>Opret, rediger, fjern vare</t>
   </si>
   <si>
@@ -81,13 +69,19 @@
     <t>Opdatering</t>
   </si>
   <si>
-    <t>Aflæsning og beregning</t>
-  </si>
-  <si>
-    <t>Opdatering, aflæsning og beregning</t>
-  </si>
-  <si>
-    <t>Opdatering og aflæsning</t>
+    <t>Email faktura/ordre/kontoudtog/provisionsseddel</t>
+  </si>
+  <si>
+    <t>Opret PDF af ordre/faktura/kontoudtog/provisionsseddel</t>
+  </si>
+  <si>
+    <t>Beregning</t>
+  </si>
+  <si>
+    <t>Eksporter kommaseparerede filer</t>
+  </si>
+  <si>
+    <t>Udregn priser på ordrer(total, total+moms)</t>
   </si>
 </sst>
 </file>
@@ -266,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,15 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,13 +284,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -609,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,177 +623,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="C15" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Beskrivelse af komplekse operationer og opdatering af funktionsliste
</commit_message>
<xml_diff>
--- a/System udvikling/Funktionsliste.xlsx
+++ b/System udvikling/Funktionsliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Funktionsliste</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Opdatering</t>
-  </si>
-  <si>
-    <t>Email faktura/ordre/kontoudtog/provisionsseddel</t>
   </si>
   <si>
     <t>Opret PDF af ordre/faktura/kontoudtog/provisionsseddel</t>
@@ -287,15 +284,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -306,6 +294,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -609,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,11 +620,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -645,7 +642,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>16</v>
@@ -659,7 +656,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -670,7 +667,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,7 +675,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
@@ -700,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>16</v>
@@ -730,61 +727,50 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>